<commit_message>
little chenge in plan for AMSC
</commit_message>
<xml_diff>
--- a/Plan/2022-23/ProgrammaOrario-AMSC-22-23.xlsx
+++ b/Plan/2022-23/ProgrammaOrario-AMSC-22-23.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="73">
   <si>
     <t xml:space="preserve">Martedi</t>
   </si>
@@ -92,36 +92,33 @@
     <t xml:space="preserve">LF indisponibile</t>
   </si>
   <si>
+    <t xml:space="preserve">Classi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lauree Magistrali</t>
+  </si>
+  <si>
     <t xml:space="preserve">Classi + smart pointers</t>
   </si>
   <si>
-    <t xml:space="preserve">0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lauree Magistrali</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STL </t>
-  </si>
-  <si>
     <t xml:space="preserve">Esempi con classi e polym</t>
   </si>
   <si>
-    <t xml:space="preserve">Operators</t>
+    <t xml:space="preserve">STL intro</t>
   </si>
   <si>
     <t xml:space="preserve">Esempi STL</t>
   </si>
   <si>
-    <t xml:space="preserve">Completamento parte C++</t>
+    <t xml:space="preserve">Operator + parallel</t>
   </si>
   <si>
     <t xml:space="preserve">MPI</t>
   </si>
   <si>
-    <t xml:space="preserve">NON C’e` Matteo</t>
-  </si>
-  <si>
     <t xml:space="preserve">Festa</t>
   </si>
   <si>
@@ -165,9 +162,6 @@
   </si>
   <si>
     <t xml:space="preserve">Classes </t>
-  </si>
-  <si>
-    <t xml:space="preserve">STL intro</t>
   </si>
   <si>
     <t xml:space="preserve">Into Parallel</t>
@@ -453,7 +447,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -512,12 +506,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB2B2B2"/>
         <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
     <fill>
@@ -674,7 +662,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="86">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -867,6 +855,70 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -879,11 +931,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="24" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="17" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="22" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -891,82 +951,6 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="16" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="17" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1003,23 +987,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="15" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="15" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="17" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="13" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="14" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="14" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1119,8 +1103,8 @@
   </sheetPr>
   <dimension ref="A1:AA55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K23" activeCellId="0" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1859,12 +1843,11 @@
         <f aca="false">H16+E17</f>
         <v>8</v>
       </c>
-      <c r="I17" s="0"/>
+      <c r="I17" s="1"/>
       <c r="J17" s="9"/>
       <c r="K17" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="M17" s="0"/>
       <c r="N17" s="9"/>
       <c r="O17" s="9"/>
       <c r="P17" s="9"/>
@@ -1957,31 +1940,29 @@
         <f aca="false">H18+E19</f>
         <v>8</v>
       </c>
-      <c r="I19" s="20" t="s">
+      <c r="I19" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="J19" s="53"/>
-      <c r="K19" s="54"/>
-      <c r="L19" s="55" t="s">
-        <v>31</v>
-      </c>
-      <c r="M19" s="53"/>
-      <c r="N19" s="53"/>
-      <c r="O19" s="53"/>
-      <c r="P19" s="53"/>
-      <c r="Q19" s="53"/>
-      <c r="R19" s="53"/>
-      <c r="S19" s="53"/>
-      <c r="T19" s="53"/>
-      <c r="U19" s="53"/>
-      <c r="V19" s="53"/>
-      <c r="W19" s="53"/>
-      <c r="X19" s="53"/>
-      <c r="Y19" s="53"/>
-      <c r="Z19" s="53"/>
-      <c r="AA19" s="53"/>
-    </row>
-    <row r="20" s="60" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J19" s="54"/>
+      <c r="K19" s="55"/>
+      <c r="L19" s="56"/>
+      <c r="M19" s="54"/>
+      <c r="N19" s="54"/>
+      <c r="O19" s="54"/>
+      <c r="P19" s="54"/>
+      <c r="Q19" s="54"/>
+      <c r="R19" s="54"/>
+      <c r="S19" s="54"/>
+      <c r="T19" s="54"/>
+      <c r="U19" s="54"/>
+      <c r="V19" s="54"/>
+      <c r="W19" s="54"/>
+      <c r="X19" s="54"/>
+      <c r="Y19" s="54"/>
+      <c r="Z19" s="54"/>
+      <c r="AA19" s="54"/>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="35" t="s">
         <v>13</v>
       </c>
@@ -1994,11 +1975,11 @@
       </c>
       <c r="D20" s="37"/>
       <c r="E20" s="37"/>
-      <c r="F20" s="56" t="n">
+      <c r="F20" s="57" t="n">
         <f aca="false">F19+C20</f>
         <v>24</v>
       </c>
-      <c r="G20" s="56" t="n">
+      <c r="G20" s="57" t="n">
         <f aca="false">G19+D20</f>
         <v>20</v>
       </c>
@@ -2006,11 +1987,11 @@
         <f aca="false">H19+E20</f>
         <v>8</v>
       </c>
-      <c r="I20" s="57"/>
-      <c r="J20" s="57"/>
-      <c r="K20" s="58"/>
-      <c r="L20" s="59" t="s">
-        <v>32</v>
+      <c r="I20" s="58"/>
+      <c r="J20" s="58"/>
+      <c r="K20" s="59"/>
+      <c r="L20" s="60" t="s">
+        <v>31</v>
       </c>
       <c r="M20" s="40"/>
       <c r="N20" s="40"/>
@@ -2060,7 +2041,7 @@
       <c r="I21" s="11"/>
       <c r="J21" s="8"/>
       <c r="K21" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L21" s="7"/>
       <c r="M21" s="9"/>
@@ -2092,11 +2073,11 @@
       </c>
       <c r="D22" s="37"/>
       <c r="E22" s="37"/>
-      <c r="F22" s="56" t="n">
+      <c r="F22" s="57" t="n">
         <f aca="false">F21+C22</f>
         <v>26</v>
       </c>
-      <c r="G22" s="56" t="n">
+      <c r="G22" s="57" t="n">
         <f aca="false">G21+D22</f>
         <v>20</v>
       </c>
@@ -2105,10 +2086,10 @@
         <v>10</v>
       </c>
       <c r="I22" s="41"/>
-      <c r="J22" s="57"/>
-      <c r="K22" s="57"/>
+      <c r="J22" s="58"/>
+      <c r="K22" s="58"/>
       <c r="L22" s="62" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M22" s="63"/>
       <c r="N22" s="40"/>
@@ -2155,7 +2136,7 @@
       </c>
       <c r="J23" s="8"/>
       <c r="K23" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M23" s="9"/>
       <c r="N23" s="9"/>
@@ -2201,7 +2182,7 @@
         <v>12</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J24" s="8"/>
       <c r="K24" s="43"/>
@@ -2298,7 +2279,7 @@
         <v>14</v>
       </c>
       <c r="I26" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J26" s="8"/>
       <c r="L26" s="7"/>
@@ -2366,7 +2347,7 @@
       <c r="Z27" s="9"/>
       <c r="AA27" s="9"/>
     </row>
-    <row r="28" s="72" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="64" t="s">
         <v>13</v>
       </c>
@@ -2445,24 +2426,24 @@
         <v>20</v>
       </c>
       <c r="I29" s="3"/>
-      <c r="J29" s="73"/>
-      <c r="K29" s="73"/>
+      <c r="J29" s="72"/>
+      <c r="K29" s="72"/>
       <c r="L29" s="4"/>
-      <c r="M29" s="74"/>
-      <c r="N29" s="74"/>
-      <c r="O29" s="74"/>
-      <c r="P29" s="74"/>
-      <c r="Q29" s="74"/>
-      <c r="R29" s="74"/>
-      <c r="S29" s="74"/>
-      <c r="T29" s="74"/>
-      <c r="U29" s="74"/>
-      <c r="V29" s="74"/>
-      <c r="W29" s="74"/>
-      <c r="X29" s="74"/>
-      <c r="Y29" s="74"/>
-      <c r="Z29" s="74"/>
-      <c r="AA29" s="74"/>
+      <c r="M29" s="73"/>
+      <c r="N29" s="73"/>
+      <c r="O29" s="73"/>
+      <c r="P29" s="73"/>
+      <c r="Q29" s="73"/>
+      <c r="R29" s="73"/>
+      <c r="S29" s="73"/>
+      <c r="T29" s="73"/>
+      <c r="U29" s="73"/>
+      <c r="V29" s="73"/>
+      <c r="W29" s="73"/>
+      <c r="X29" s="73"/>
+      <c r="Y29" s="73"/>
+      <c r="Z29" s="73"/>
+      <c r="AA29" s="73"/>
     </row>
     <row r="30" s="20" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="20" t="s">
@@ -2535,10 +2516,10 @@
         <v>20</v>
       </c>
       <c r="I31" s="41"/>
-      <c r="J31" s="75"/>
-      <c r="K31" s="76"/>
-      <c r="L31" s="59" t="s">
-        <v>32</v>
+      <c r="J31" s="74"/>
+      <c r="K31" s="75"/>
+      <c r="L31" s="60" t="s">
+        <v>31</v>
       </c>
       <c r="M31" s="40"/>
       <c r="N31" s="40"/>
@@ -2663,11 +2644,11 @@
       </c>
       <c r="D34" s="37"/>
       <c r="E34" s="37"/>
-      <c r="F34" s="56" t="n">
+      <c r="F34" s="57" t="n">
         <f aca="false">F33+C34</f>
         <v>46</v>
       </c>
-      <c r="G34" s="56" t="n">
+      <c r="G34" s="57" t="n">
         <f aca="false">G33+D34</f>
         <v>30</v>
       </c>
@@ -2676,10 +2657,10 @@
         <v>20</v>
       </c>
       <c r="I34" s="41"/>
-      <c r="J34" s="57"/>
-      <c r="K34" s="57"/>
-      <c r="L34" s="59" t="s">
-        <v>38</v>
+      <c r="J34" s="58"/>
+      <c r="K34" s="58"/>
+      <c r="L34" s="60" t="s">
+        <v>37</v>
       </c>
       <c r="M34" s="40"/>
       <c r="N34" s="40"/>
@@ -2744,13 +2725,13 @@
       <c r="AA35" s="9"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="77"/>
-      <c r="C36" s="78"/>
-      <c r="D36" s="78"/>
-      <c r="E36" s="78"/>
-      <c r="F36" s="79"/>
-      <c r="G36" s="79"/>
-      <c r="H36" s="79"/>
+      <c r="B36" s="76"/>
+      <c r="C36" s="77"/>
+      <c r="D36" s="77"/>
+      <c r="E36" s="77"/>
+      <c r="F36" s="78"/>
+      <c r="G36" s="78"/>
+      <c r="H36" s="78"/>
       <c r="I36" s="8"/>
       <c r="J36" s="8"/>
       <c r="K36" s="8"/>
@@ -2772,7 +2753,7 @@
       <c r="AA36" s="9"/>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B37" s="80"/>
+      <c r="B37" s="79"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
@@ -2800,7 +2781,7 @@
       <c r="AA37" s="9"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="80"/>
+      <c r="B38" s="79"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
@@ -2812,51 +2793,51 @@
       <c r="K38" s="8"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="77"/>
-      <c r="C39" s="78"/>
-      <c r="D39" s="78"/>
-      <c r="E39" s="78"/>
-      <c r="F39" s="79"/>
-      <c r="G39" s="79"/>
-      <c r="H39" s="79"/>
+      <c r="B39" s="76"/>
+      <c r="C39" s="77"/>
+      <c r="D39" s="77"/>
+      <c r="E39" s="77"/>
+      <c r="F39" s="78"/>
+      <c r="G39" s="78"/>
+      <c r="H39" s="78"/>
       <c r="J39" s="8"/>
       <c r="K39" s="8"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C40" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F40" s="81" t="n">
+        <v>38</v>
+      </c>
+      <c r="F40" s="80" t="n">
         <v>32</v>
       </c>
-      <c r="G40" s="81" t="n">
+      <c r="G40" s="80" t="n">
         <f aca="false">F40/2</f>
         <v>16</v>
       </c>
-      <c r="H40" s="81"/>
+      <c r="H40" s="80"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C41" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F41" s="81" t="n">
+      <c r="F41" s="80" t="n">
         <v>18</v>
       </c>
-      <c r="G41" s="81" t="n">
+      <c r="G41" s="80" t="n">
         <f aca="false">F41/2</f>
         <v>9</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F42" s="1" t="n">
         <f aca="false">F41+F40</f>
         <v>50</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K42" s="3" t="n">
         <v>21</v>
@@ -2867,7 +2848,7 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I43" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K43" s="3" t="n">
         <v>91</v>
@@ -2891,7 +2872,7 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I45" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K45" s="3" t="n">
         <v>31</v>
@@ -2903,7 +2884,7 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I46" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K46" s="3" t="n">
         <v>40</v>
@@ -2915,7 +2896,7 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I47" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K47" s="3" t="n">
         <v>12</v>
@@ -2927,7 +2908,7 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I48" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K48" s="3" t="n">
         <v>78</v>
@@ -2939,7 +2920,7 @@
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I49" s="3" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="K49" s="3" t="n">
         <v>69</v>
@@ -2951,7 +2932,7 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I50" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K50" s="3" t="n">
         <v>20</v>
@@ -2975,7 +2956,7 @@
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I52" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K52" s="3" t="n">
         <v>36</v>
@@ -3041,116 +3022,116 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="81" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="81" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="82" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="82" t="s">
+      <c r="B2" s="83" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="83" t="s">
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="82" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="84" t="s">
+      <c r="B3" s="84" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="83" t="s">
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="84" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="85" t="s">
+      <c r="B4" s="84" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="85" t="s">
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="84" t="s">
         <v>56</v>
       </c>
-      <c r="B4" s="85" t="s">
+      <c r="B5" s="84" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="85" t="s">
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="84" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="85" t="s">
+      <c r="B6" s="84" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="85" t="s">
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B7" s="84" t="s">
         <v>60</v>
       </c>
-      <c r="B6" s="85" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B8" s="85" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="85" t="s">
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B9" s="84" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="86" t="s">
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B10" s="84" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="85" t="s">
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B11" s="85" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="85" t="s">
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B12" s="84" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="86" t="s">
+    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B13" s="84" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="85" t="s">
+    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B14" s="84" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="85" t="s">
+    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B15" s="84" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="85" t="s">
+    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B16" s="85" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="85" t="s">
+    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B17" s="84" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="86" t="s">
+    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B18" s="85" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="85" t="s">
+    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B19" s="84" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B18" s="86" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B19" s="85" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>